<commit_message>
add size in BIT STRING need to process in jinja
</commit_message>
<xml_diff>
--- a/data_xlsx/data_excel.xlsx
+++ b/data_xlsx/data_excel.xlsx
@@ -1863,7 +1863,7 @@
       </c>
       <c r="F29" s="1" t="inlineStr">
         <is>
-          <t>BIT STRING</t>
+          <t>BIT STRING (SIZE (20)</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1904,7 +1904,7 @@
       </c>
       <c r="F30" s="1" t="inlineStr">
         <is>
-          <t>BIT STRING</t>
+          <t>BIT STRING (SIZE (28)</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="F31" s="1" t="inlineStr">
         <is>
-          <t>BIT STRING</t>
+          <t>BIT STRING (SIZE(18)</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="F32" s="1" t="inlineStr">
         <is>
-          <t>BIT STRING</t>
+          <t>BIT STRING (SIZE(21)</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="F33" s="1" t="inlineStr">
         <is>
-          <t>BIT STRING</t>
+          <t>BIT STRING (SIZE(20)</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -2068,7 +2068,7 @@
       </c>
       <c r="F34" s="1" t="inlineStr">
         <is>
-          <t>BIT STRING</t>
+          <t>BIT STRING (SIZE(18)</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="F35" s="1" t="inlineStr">
         <is>
-          <t>BIT STRING</t>
+          <t>BIT STRING (SIZE(21)</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -2150,7 +2150,7 @@
       </c>
       <c r="F36" s="1" t="inlineStr">
         <is>
-          <t>BIT STRING</t>
+          <t>BIT STRING (SIZE (22..32)</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="F37" s="1" t="inlineStr">
         <is>
-          <t>BIT STRING</t>
+          <t>BIT STRING (SIZE(22..32)</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>

</xml_diff>

<commit_message>
update some fix msg
</commit_message>
<xml_diff>
--- a/data_xlsx/data_excel.xlsx
+++ b/data_xlsx/data_excel.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,10 +426,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="19" customWidth="1" min="1" max="1"/>
-    <col width="23" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="37" customWidth="1" min="2" max="2"/>
     <col width="5" customWidth="1" min="3" max="3"/>
-    <col width="5" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="80" customWidth="1" min="5" max="5"/>
     <col width="9" customWidth="1" min="6" max="6"/>
     <col width="14" customWidth="1" min="7" max="7"/>
@@ -475,19 +475,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CauseE2node</t>
+          <t>AMFName</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ENUMERATED</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>[(0,"e2node-component-unknown","e2node-component-unknown")]</t>
-        </is>
-      </c>
+          <t>PrintableString (SIZE(1..150, ...))</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
           <t>1</t>
@@ -502,7 +508,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CauseMisc</t>
+          <t>E2nodeComponentInterfaceType</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -512,7 +518,7 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>[(0,"control-processing-overload","control-processing-overload"),(1,"hardware-failure","hardware-failure"),(2,"om-intervention","om-intervention"),(3,"unspecified","unspecified")]</t>
+          <t>[(0,"ng","ng"),(1,"xn","xn"),(2,"e1","e1"),(3,"f1","f1"),(4,"w1","w1"),(5,"s1","s1"),(6,"x2","x2")]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -529,22 +535,28 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CauseProtocol</t>
+          <t>GNB-CU-UP-ID</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ENUMERATED</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>[(0,"transfer-syntax-error","transfer-syntax-error"),(1,"abstract-syntax-error-reject","abstract-syntax-error-reject"),(2,"abstract-syntax-error-ignore-and-notify","abstract-syntax-error-ignore-and-notify"),(3,"message-not-compatible-with-receiver-state","message-not-compatible-with-receiver-state"),(4,"semantic-error","semantic-error"),(5,"abstract-syntax-error-falsely-constructed-message","abstract-syntax-error-falsely-constructed-message"),(6,"unspecified","unspecified")]</t>
-        </is>
-      </c>
+          <t>INTEGER (0..68719476735)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>68719476735</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -556,22 +568,28 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CauseRICrequest</t>
+          <t>GNB-DU-ID</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ENUMERATED</t>
-        </is>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>[(0,"ran-function-id-invalid","ran-function-id-invalid"),(1,"action-not-supported","action-not-supported"),(2,"excessive-actions","excessive-actions"),(3,"duplicate-action","duplicate-action"),(4,"duplicate-event-trigger","duplicate-event-trigger"),(5,"function-resource-limit","function-resource-limit"),(6,"request-id-unknown","request-id-unknown"),(7,"inconsistent-action-subsequent-action-sequence","inconsistent-action-subsequent-action-sequence"),(8,"control-message-invalid","control-message-invalid"),(9,"ric-call-process-id-invalid","ric-call-process-id-invalid"),(10,"control-timer-expired","control-timer-expired"),(11,"control-failed-to-execute","control-failed-to-execute"),(12,"system-not-ready","system-not-ready"),(13,"unspecified","unspecified"),(14,"ric-subscription-end-time-expired","ric-subscription-end-time-expired"),(15,"ric-subscription-end-time-invalid","ric-subscription-end-time-invalid"),(16,"duplicate-ric-request-id","duplicate-ric-request-id"),(17,"eventTriggerNotSupported","eventTriggerNotSupported"),(18,"requested-information-unavailable","requested-information-unavailable"),(19,"invalid-information-request","invalid-information-request")]</t>
-        </is>
-      </c>
+          <t>INTEGER (0..68719476735)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>68719476735</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -583,22 +601,28 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CauseRICservice</t>
+          <t>NGENB-DU-ID</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ENUMERATED</t>
-        </is>
-      </c>
-      <c r="E6" s="1" t="inlineStr">
-        <is>
-          <t>[(0,"ran-function-not-supported","ran-function-not-supported"),(1,"excessive-functions","excessive-functions"),(2,"ric-resource-limit","ric-resource-limit")]</t>
-        </is>
-      </c>
+          <t>INTEGER (0..68719476735)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>68719476735</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -610,46 +634,38 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CauseTransport</t>
+          <t>PLMN-Identity</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ENUMERATED</t>
-        </is>
-      </c>
-      <c r="E7" s="1" t="inlineStr">
-        <is>
-          <t>[(0,"unspecified","unspecified"),(1,"transport-resource-unavailable","transport-resource-unavailable")]</t>
-        </is>
-      </c>
+          <t>OCTET STRING (SIZE(3))</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Criticality</t>
+          <t>RANfunctionDefinition</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ENUMERATED</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="inlineStr">
-        <is>
-          <t>[(0,"reject","reject"),(1,"ignore","ignore"),(2,"notify","notify")]</t>
-        </is>
-      </c>
+          <t>OCTET STRING</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>0</t>
@@ -664,12 +680,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ProcedureCode</t>
+          <t>RANfunctionID</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>INTEGER (0..255)</t>
+          <t>INTEGER (0..4095)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -679,7 +695,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>255</t>
+          <t>4095</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr"/>
@@ -697,18 +713,28 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ServiceLayerCause</t>
+          <t>RANfunctionOID</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>OCTET STRING</t>
+          <t>PrintableString (SIZE(1..1000,...))</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1000</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -720,22 +746,28 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TimeToWait</t>
+          <t>RANfunctionRevision</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ENUMERATED</t>
-        </is>
-      </c>
-      <c r="E11" s="1" t="inlineStr">
-        <is>
-          <t>[(0,"v1s","v1s"),(1,"v2s","v2s"),(2,"v5s","v5s"),(3,"v10s","v10s"),(4,"v20s","v20s"),(5,"v60s","v60s")]</t>
-        </is>
-      </c>
+          <t>INTEGER (0..4095)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>4095</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -772,33 +804,6 @@
         </is>
       </c>
       <c r="G12" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>TriggeringMessage</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>ENUMERATED</t>
-        </is>
-      </c>
-      <c r="E13" s="1" t="inlineStr">
-        <is>
-          <t>[(0,"initiating-message","initiating-message"),(1,"successful-outcome","successful-outcome"),(2,"unsuccessfull-outcome","unsuccessfull-outcome")]</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
@@ -815,7 +820,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -823,17 +828,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="32" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="32" customWidth="1" min="3" max="3"/>
+    <col width="39" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="2" max="2"/>
+    <col width="39" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
-    <col width="27" customWidth="1" min="5" max="5"/>
-    <col width="32" customWidth="1" min="6" max="6"/>
+    <col width="39" customWidth="1" min="5" max="5"/>
+    <col width="39" customWidth="1" min="6" max="6"/>
     <col width="13" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
     <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
+    <col width="23" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -896,32 +901,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cause</t>
+          <t>E2nodeComponentConfigAddition-Item</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CHOICE</t>
+          <t>SEQUENCE</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cause</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+          <t>E2nodeComponentConfigAddition-Item</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>ricRequest</t>
+          <t>e2nodeComponentInterfaceType</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>CauseRICrequest</t>
+          <t>E2nodeComponentInterfaceType</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -937,32 +938,28 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cause</t>
+          <t>E2nodeComponentConfigAddition-Item</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CHOICE</t>
+          <t>SEQUENCE</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Cause</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>E2nodeComponentConfigAddition-Item</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>ricService</t>
+          <t>e2nodeComponentID</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>CauseRICservice</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -978,32 +975,28 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cause</t>
+          <t>E2nodeComponentConfigAddition-Item</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CHOICE</t>
+          <t>SEQUENCE</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Cause</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+          <t>E2nodeComponentConfigAddition-Item</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>e2Node</t>
+          <t>e2nodeComponentConfiguration</t>
         </is>
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>CauseE2node</t>
+          <t>E2nodeComponentConfiguration</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -1019,35 +1012,35 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cause</t>
+          <t>E2nodeComponentConfigAddition-ItemIEs</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CHOICE</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Cause</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+          <t>E2nodeComponentConfigAddition-ItemIEs</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>id-E2nodeComponentConfigAddition-Item</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>CauseTransport</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
+          <t>E2nodeComponentConfigAddition-Item</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
@@ -1060,73 +1053,69 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cause</t>
+          <t>E2nodeComponentConfigAddition-List</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CHOICE</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Cause</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+          <t>SingleContainer</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>protocol</t>
+          <t>E2nodeComponentConfigAddition-List</t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>CauseProtocol</t>
+          <t>E2nodeComponentConfigAddition-ItemIEs</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>maxofE2nodeComponents</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cause</t>
+          <t>E2nodeComponentConfiguration</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CHOICE</t>
+          <t>SEQUENCE</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Cause</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+          <t>E2nodeComponentConfiguration</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>e2nodeComponentRequestPart</t>
         </is>
       </c>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>CauseMisc</t>
+          <t>e2nodeComponentRequestPart</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -1142,32 +1131,28 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cause</t>
+          <t>E2nodeComponentConfiguration</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CHOICE</t>
+          <t>SEQUENCE</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Cause</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
+          <t>E2nodeComponentConfiguration</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>serviceLayer</t>
+          <t>e2nodeComponentResponsePart</t>
         </is>
       </c>
       <c r="F8" s="1" t="inlineStr">
         <is>
-          <t>CauseServiceLayer</t>
+          <t>e2nodeComponentResponsePart</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -1183,28 +1168,32 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CauseServiceLayer</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CauseServiceLayer</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>serviceLayerCause</t>
+          <t>e2nodeComponentInterfaceTypeNG</t>
         </is>
       </c>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>ServiceLayerCause</t>
+          <t>E2nodeComponentInterfaceNG</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -1220,36 +1209,36 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>procedureCode</t>
+          <t>e2nodeComponentInterfaceTypeXn</t>
         </is>
       </c>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>ProcedureCode</t>
+          <t>E2nodeComponentInterfaceXn</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
           <t>1</t>
@@ -1261,36 +1250,36 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>triggeringMessage</t>
+          <t>e2nodeComponentInterfaceTypeE1</t>
         </is>
       </c>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>TriggeringMessage</t>
+          <t>E2nodeComponentInterfaceE1</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
           <t>1</t>
@@ -1302,36 +1291,36 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>procedureCriticality</t>
+          <t>e2nodeComponentInterfaceTypeF1</t>
         </is>
       </c>
       <c r="F12" s="1" t="inlineStr">
         <is>
-          <t>Criticality</t>
+          <t>E2nodeComponentInterfaceF1</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
           <t>1</t>
@@ -1343,36 +1332,36 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>ricRequestorID</t>
+          <t>e2nodeComponentInterfaceTypeW1</t>
         </is>
       </c>
       <c r="F13" s="1" t="inlineStr">
         <is>
-          <t>RICrequestID</t>
+          <t>E2nodeComponentInterfaceW1</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
           <t>1</t>
@@ -1384,36 +1373,36 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>iEsCriticalityDiagnostics</t>
+          <t>e2nodeComponentInterfaceTypeS1</t>
         </is>
       </c>
       <c r="F14" s="1" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
+          <t>E2nodeComponentInterfaceS1</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
           <t>1</t>
@@ -1425,28 +1414,32 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>iECriticality</t>
+          <t>e2nodeComponentInterfaceTypeX2</t>
         </is>
       </c>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>Criticality</t>
+          <t>E2nodeComponentInterfaceX2</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -1462,7 +1455,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
+          <t>E2nodeComponentInterfaceE1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1472,18 +1465,18 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
+          <t>E2nodeComponentInterfaceE1</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" s="1" t="inlineStr">
         <is>
-          <t>iE-ID</t>
+          <t>gNB-CU-UP-ID</t>
         </is>
       </c>
       <c r="F16" s="1" t="inlineStr">
         <is>
-          <t>ProtocolIE-ID</t>
+          <t>GNB-CU-UP-ID</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
@@ -1499,7 +1492,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
+          <t>E2nodeComponentInterfaceF1</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1509,18 +1502,18 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
+          <t>E2nodeComponentInterfaceF1</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>typeOfError</t>
+          <t>gNB-DU-ID</t>
         </is>
       </c>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>TypeOfError</t>
+          <t>GNB-DU-ID</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -1536,7 +1529,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>E2setupFailure</t>
+          <t>E2nodeComponentInterfaceNG</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1546,18 +1539,18 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>E2setupFailure</t>
+          <t>E2nodeComponentInterfaceNG</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" s="1" t="inlineStr">
         <is>
-          <t>protocolIEs</t>
+          <t>amf-name</t>
         </is>
       </c>
       <c r="F18" s="1" t="inlineStr">
         <is>
-          <t>ProtocolIE-Container</t>
+          <t>AMFName</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1573,35 +1566,31 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2nodeComponentInterfaceS1</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>SEQUENCE</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2nodeComponentInterfaceS1</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>id-TransactionID</t>
+          <t>mme-name</t>
         </is>
       </c>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>TransactionID</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>reject</t>
-        </is>
-      </c>
+          <t>MMEname</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
@@ -1614,35 +1603,31 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2nodeComponentInterfaceW1</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>SEQUENCE</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2nodeComponentInterfaceW1</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" s="1" t="inlineStr">
         <is>
-          <t>id-TransactionID</t>
+          <t>ng-eNB-DU-ID</t>
         </is>
       </c>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>Cause</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>reject</t>
-        </is>
-      </c>
+          <t>NGENB-DU-ID</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
@@ -1655,36 +1640,36 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2nodeComponentInterfaceX2</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>SEQUENCE</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2nodeComponentInterfaceX2</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" s="1" t="inlineStr">
         <is>
-          <t>id-TransactionID</t>
+          <t>global-eNB-ID</t>
         </is>
       </c>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>TimeToWait</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>reject</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr">
         <is>
           <t>1</t>
@@ -1696,36 +1681,36 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2nodeComponentInterfaceX2</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>SEQUENCE</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2nodeComponentInterfaceX2</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" s="1" t="inlineStr">
         <is>
-          <t>id-TransactionID</t>
+          <t>global-en-gNB-ID</t>
         </is>
       </c>
       <c r="F22" s="1" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>reject</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr"/>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
       <c r="I22" t="inlineStr">
         <is>
           <t>1</t>
@@ -1737,35 +1722,31 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2nodeComponentInterfaceXn</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>SEQUENCE</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2nodeComponentInterfaceXn</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" s="1" t="inlineStr">
         <is>
-          <t>id-TransactionID</t>
+          <t>global-NG-RAN-Node-ID</t>
         </is>
       </c>
       <c r="F23" s="1" t="inlineStr">
         <is>
-          <t>TNLinformation</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>reject</t>
-        </is>
-      </c>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
         <is>
@@ -1778,7 +1759,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>RICrequestID</t>
+          <t>E2setupRequest</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1788,18 +1769,18 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>RICrequestID</t>
+          <t>E2setupRequest</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" s="1" t="inlineStr">
         <is>
-          <t>ricRequestorID</t>
+          <t>protocolIEs</t>
         </is>
       </c>
       <c r="F24" s="1" t="inlineStr">
         <is>
-          <t>ricRequestorID</t>
+          <t>ProtocolIE-Container</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -1815,31 +1796,35 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>RICrequestID</t>
+          <t>E2setupRequestIEs</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>RICrequestID</t>
+          <t>E2setupRequestIEs</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" s="1" t="inlineStr">
         <is>
-          <t>ricInstanceID</t>
+          <t>id-TransactionID</t>
         </is>
       </c>
       <c r="F25" s="1" t="inlineStr">
         <is>
-          <t>ricInstanceID</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr"/>
+          <t>TransactionID</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr">
         <is>
@@ -1852,31 +1837,35 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>TNLinformation</t>
+          <t>E2setupRequestIEs</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>TNLinformation</t>
+          <t>E2setupRequestIEs</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" s="1" t="inlineStr">
         <is>
-          <t>tnlAddress</t>
+          <t>id-GlobalE2node-ID</t>
         </is>
       </c>
       <c r="F26" s="1" t="inlineStr">
         <is>
-          <t>BIT STRING (SIZE(1..160,...)</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr"/>
+          <t>GlobalE2node-ID</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr">
         <is>
@@ -1889,36 +1878,36 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>TNLinformation</t>
+          <t>E2setupRequestIEs</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>TNLinformation</t>
+          <t>E2setupRequestIEs</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" s="1" t="inlineStr">
         <is>
-          <t>tnlPort</t>
+          <t>id-RANfunctionsAdded</t>
         </is>
       </c>
       <c r="F27" s="1" t="inlineStr">
         <is>
-          <t>BIT STRING (SIZE(16)</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+          <t>RANfunctions-List</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
           <t>1</t>
@@ -1926,6 +1915,1623 @@
       </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>E2setupRequestIEs</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>E2setupRequestIEs</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" s="1" t="inlineStr">
+        <is>
+          <t>id-E2nodeComponentConfigAddition</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigAddition-List</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E29" s="1" t="inlineStr">
+        <is>
+          <t>macro-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F29" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE (20)</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E30" s="1" t="inlineStr">
+        <is>
+          <t>home-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F30" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE (28)</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E31" s="1" t="inlineStr">
+        <is>
+          <t>short-Macro-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F31" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(18)</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E32" s="1" t="inlineStr">
+        <is>
+          <t>long-Macro-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F32" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(21)</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E33" s="1" t="inlineStr">
+        <is>
+          <t>enb-ID-macro</t>
+        </is>
+      </c>
+      <c r="F33" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(20)</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E34" s="1" t="inlineStr">
+        <is>
+          <t>enb-ID-shortmacro</t>
+        </is>
+      </c>
+      <c r="F34" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(18)</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E35" s="1" t="inlineStr">
+        <is>
+          <t>enb-ID-longmacro</t>
+        </is>
+      </c>
+      <c r="F35" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(21)</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>ENGNB-ID</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ENGNB-ID</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E36" s="1" t="inlineStr">
+        <is>
+          <t>gNB-ID</t>
+        </is>
+      </c>
+      <c r="F36" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE (22..32)</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>GNB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>GNB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E37" s="1" t="inlineStr">
+        <is>
+          <t>gnb-ID</t>
+        </is>
+      </c>
+      <c r="F37" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(22..32)</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ID</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ID</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E38" s="1" t="inlineStr">
+        <is>
+          <t>gNB</t>
+        </is>
+      </c>
+      <c r="F38" s="1" t="inlineStr">
+        <is>
+          <t>GlobalE2node-gNB-ID</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ID</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ID</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E39" s="1" t="inlineStr">
+        <is>
+          <t>en-gNB</t>
+        </is>
+      </c>
+      <c r="F39" s="1" t="inlineStr">
+        <is>
+          <t>GlobalE2node-en-gNB-ID</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ID</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ID</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E40" s="1" t="inlineStr">
+        <is>
+          <t>ng-eNB</t>
+        </is>
+      </c>
+      <c r="F40" s="1" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ng-eNB-ID</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ID</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ID</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E41" s="1" t="inlineStr">
+        <is>
+          <t>eNB</t>
+        </is>
+      </c>
+      <c r="F41" s="1" t="inlineStr">
+        <is>
+          <t>GlobalE2node-eNB-ID</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>GlobalE2node-eNB-ID</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>GlobalE2node-eNB-ID</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" s="1" t="inlineStr">
+        <is>
+          <t>global-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F42" s="1" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>GlobalE2node-en-gNB-ID</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>GlobalE2node-en-gNB-ID</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" s="1" t="inlineStr">
+        <is>
+          <t>global-en-gNB-ID</t>
+        </is>
+      </c>
+      <c r="F43" s="1" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>GlobalE2node-en-gNB-ID</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>GlobalE2node-en-gNB-ID</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" s="1" t="inlineStr">
+        <is>
+          <t>en-gNB-CU-UP-ID</t>
+        </is>
+      </c>
+      <c r="F44" s="1" t="inlineStr">
+        <is>
+          <t>GNB-CU-UP-ID</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>GlobalE2node-en-gNB-ID</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>GlobalE2node-en-gNB-ID</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" s="1" t="inlineStr">
+        <is>
+          <t>en-gNB-DU-ID</t>
+        </is>
+      </c>
+      <c r="F45" s="1" t="inlineStr">
+        <is>
+          <t>GNB-DU-ID</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>GlobalE2node-gNB-ID</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>GlobalE2node-gNB-ID</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" s="1" t="inlineStr">
+        <is>
+          <t>global-gNB-ID</t>
+        </is>
+      </c>
+      <c r="F46" s="1" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>GlobalE2node-gNB-ID</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>GlobalE2node-gNB-ID</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" s="1" t="inlineStr">
+        <is>
+          <t>global-en-gNB-ID</t>
+        </is>
+      </c>
+      <c r="F47" s="1" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>GlobalE2node-gNB-ID</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>GlobalE2node-gNB-ID</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" s="1" t="inlineStr">
+        <is>
+          <t>gNB-CU-UP-ID</t>
+        </is>
+      </c>
+      <c r="F48" s="1" t="inlineStr">
+        <is>
+          <t>GNB-CU-UP-ID</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>GlobalE2node-gNB-ID</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>GlobalE2node-gNB-ID</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" s="1" t="inlineStr">
+        <is>
+          <t>gNB-DU-ID</t>
+        </is>
+      </c>
+      <c r="F49" s="1" t="inlineStr">
+        <is>
+          <t>GNB-DU-ID</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ng-eNB-ID</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ng-eNB-ID</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" s="1" t="inlineStr">
+        <is>
+          <t>global-ng-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F50" s="1" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ng-eNB-ID</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ng-eNB-ID</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" s="1" t="inlineStr">
+        <is>
+          <t>global-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F51" s="1" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ng-eNB-ID</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>GlobalE2node-ng-eNB-ID</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" s="1" t="inlineStr">
+        <is>
+          <t>ngENB-DU-ID</t>
+        </is>
+      </c>
+      <c r="F52" s="1" t="inlineStr">
+        <is>
+          <t>NGENB-DU-ID</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" s="1" t="inlineStr">
+        <is>
+          <t>pLMN-Identity</t>
+        </is>
+      </c>
+      <c r="F53" s="1" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" s="1" t="inlineStr">
+        <is>
+          <t>eNB-ID</t>
+        </is>
+      </c>
+      <c r="F54" s="1" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E55" s="1" t="inlineStr">
+        <is>
+          <t>gNB</t>
+        </is>
+      </c>
+      <c r="F55" s="1" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E56" s="1" t="inlineStr">
+        <is>
+          <t>ng-eNB</t>
+        </is>
+      </c>
+      <c r="F56" s="1" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" s="1" t="inlineStr">
+        <is>
+          <t>pLMN-Identity</t>
+        </is>
+      </c>
+      <c r="F57" s="1" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" s="1" t="inlineStr">
+        <is>
+          <t>gNB-ID</t>
+        </is>
+      </c>
+      <c r="F58" s="1" t="inlineStr">
+        <is>
+          <t>ENGNB-ID</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" s="1" t="inlineStr">
+        <is>
+          <t>plmn-id</t>
+        </is>
+      </c>
+      <c r="F59" s="1" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" s="1" t="inlineStr">
+        <is>
+          <t>gnb-id</t>
+        </is>
+      </c>
+      <c r="F60" s="1" t="inlineStr">
+        <is>
+          <t>GNB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" s="1" t="inlineStr">
+        <is>
+          <t>plmn-id</t>
+        </is>
+      </c>
+      <c r="F61" s="1" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" s="1" t="inlineStr">
+        <is>
+          <t>enb-id</t>
+        </is>
+      </c>
+      <c r="F62" s="1" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>RANfunction-Item</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>RANfunction-Item</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" s="1" t="inlineStr">
+        <is>
+          <t>ranFunctionID</t>
+        </is>
+      </c>
+      <c r="F63" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionID</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>RANfunction-Item</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>RANfunction-Item</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" s="1" t="inlineStr">
+        <is>
+          <t>ranFunctionDefinition</t>
+        </is>
+      </c>
+      <c r="F64" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionDefinition</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>RANfunction-Item</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>RANfunction-Item</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" s="1" t="inlineStr">
+        <is>
+          <t>ranFunctionRevision</t>
+        </is>
+      </c>
+      <c r="F65" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionRevision</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>RANfunction-Item</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>RANfunction-Item</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" s="1" t="inlineStr">
+        <is>
+          <t>ranFunctionOID</t>
+        </is>
+      </c>
+      <c r="F66" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionOID</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>RANfunction-ItemIEs</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>RANfunction-ItemIEs</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" s="1" t="inlineStr">
+        <is>
+          <t>id-RANfunction-Item</t>
+        </is>
+      </c>
+      <c r="F67" s="1" t="inlineStr">
+        <is>
+          <t>RANfunction-Item</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>ignore</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>RANfunctions-List</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>SingleContainer</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctions-List</t>
+        </is>
+      </c>
+      <c r="F68" s="1" t="inlineStr">
+        <is>
+          <t>RANfunction-ItemIEs</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>maxofRANfunctionID</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1938,7 +3544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1947,9 +3553,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="16" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="2" max="2"/>
-    <col width="24" customWidth="1" min="3" max="3"/>
-    <col width="24" customWidth="1" min="4" max="4"/>
+    <col width="42" customWidth="1" min="2" max="2"/>
+    <col width="36" customWidth="1" min="3" max="3"/>
+    <col width="34" customWidth="1" min="4" max="4"/>
     <col width="19" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
     <col width="11" customWidth="1" min="7" max="7"/>
@@ -1995,7 +3601,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>E2setupFailure</t>
+          <t>E2setupRequest</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2010,12 +3616,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>transactionID</t>
+          <t>id-TransactionID</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2setupRequestIEs</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2032,27 +3638,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>E2setupFailure</t>
+          <t>E2setupRequest</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ID_id_Cause</t>
+          <t>ID_id_GlobalE2node-ID</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Cause</t>
+          <t>GlobalE2node-ID</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>cause</t>
+          <t>id-GlobalE2node-ID</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2setupRequestIEs</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2069,27 +3675,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>E2setupFailure</t>
+          <t>E2setupRequest</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ID_id_TimeToWait</t>
+          <t>ID_id_RANfunctions-List</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>TimeToWait</t>
+          <t>RANfunctions-List</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>timeToWait</t>
+          <t>id-RANfunctionsAdded</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2setupRequestIEs</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -2106,27 +3712,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>E2setupFailure</t>
+          <t>E2setupRequest</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ID_id_CriticalityDiagnostics</t>
+          <t>ID_id_E2nodeComponentConfigAddition-List</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentConfigAddition-List</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>criticalityDiagnostics</t>
+          <t>id-E2nodeComponentConfigAddition</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>E2setupFailureIEs</t>
+          <t>E2setupRequestIEs</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2135,43 +3741,6 @@
         </is>
       </c>
       <c r="G5" t="inlineStr">
-        <is>
-          <t>MANDATORY</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>E2setupFailure</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ID_id_TNLinformation</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>TNLinformation</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>tNLinformation</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>E2setupFailureIEs</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>reject</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
         <is>
           <t>MANDATORY</t>
         </is>

</xml_diff>

<commit_message>
fix choice with intergratr
</commit_message>
<xml_diff>
--- a/data_xlsx/data_excel.xlsx
+++ b/data_xlsx/data_excel.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,10 +426,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="23" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="37" customWidth="1" min="2" max="2"/>
     <col width="5" customWidth="1" min="3" max="3"/>
-    <col width="5" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="80" customWidth="1" min="5" max="5"/>
     <col width="9" customWidth="1" min="6" max="6"/>
     <col width="14" customWidth="1" min="7" max="7"/>
@@ -475,19 +475,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TNLusage</t>
+          <t>AMFName</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ENUMERATED</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>[(0,"ric-service","ric-service"),(1,"support-function","support-function"),(2,"both","both")]</t>
-        </is>
-      </c>
+          <t>PrintableString (SIZE(1..150, ...))</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
           <t>1</t>
@@ -502,31 +508,365 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>CauseE2node</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ENUMERATED</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>[(0,"e2node-component-unknown","e2node-component-unknown")]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CauseMisc</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ENUMERATED</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>[(0,"control-processing-overload","control-processing-overload"),(1,"hardware-failure","hardware-failure"),(2,"om-intervention","om-intervention"),(3,"unspecified","unspecified")]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CauseProtocol</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ENUMERATED</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>[(0,"transfer-syntax-error","transfer-syntax-error"),(1,"abstract-syntax-error-reject","abstract-syntax-error-reject"),(2,"abstract-syntax-error-ignore-and-notify","abstract-syntax-error-ignore-and-notify"),(3,"message-not-compatible-with-receiver-state","message-not-compatible-with-receiver-state"),(4,"semantic-error","semantic-error"),(5,"abstract-syntax-error-falsely-constructed-message","abstract-syntax-error-falsely-constructed-message"),(6,"unspecified","unspecified")]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CauseRICrequest</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ENUMERATED</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>[(0,"ran-function-id-invalid","ran-function-id-invalid"),(1,"action-not-supported","action-not-supported"),(2,"excessive-actions","excessive-actions"),(3,"duplicate-action","duplicate-action"),(4,"duplicate-event-trigger","duplicate-event-trigger"),(5,"function-resource-limit","function-resource-limit"),(6,"request-id-unknown","request-id-unknown"),(7,"inconsistent-action-subsequent-action-sequence","inconsistent-action-subsequent-action-sequence"),(8,"control-message-invalid","control-message-invalid"),(9,"ric-call-process-id-invalid","ric-call-process-id-invalid"),(10,"control-timer-expired","control-timer-expired"),(11,"control-failed-to-execute","control-failed-to-execute"),(12,"system-not-ready","system-not-ready"),(13,"unspecified","unspecified"),(14,"ric-subscription-end-time-expired","ric-subscription-end-time-expired"),(15,"ric-subscription-end-time-invalid","ric-subscription-end-time-invalid"),(16,"duplicate-ric-request-id","duplicate-ric-request-id"),(17,"eventTriggerNotSupported","eventTriggerNotSupported"),(18,"requested-information-unavailable","requested-information-unavailable"),(19,"invalid-information-request","invalid-information-request")]</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CauseRICservice</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ENUMERATED</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
+          <t>[(0,"ran-function-not-supported","ran-function-not-supported"),(1,"excessive-functions","excessive-functions"),(2,"ric-resource-limit","ric-resource-limit")]</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CauseTransport</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ENUMERATED</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>[(0,"unspecified","unspecified"),(1,"transport-resource-unavailable","transport-resource-unavailable")]</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceType</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ENUMERATED</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>[(0,"ng","ng"),(1,"xn","xn"),(2,"e1","e1"),(3,"f1","f1"),(4,"w1","w1"),(5,"s1","s1"),(6,"x2","x2")]</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>GNB-CU-UP-ID</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>INTEGER (0..68719476735)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>68719476735</t>
+        </is>
+      </c>
+      <c r="E10" s="1" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>GNB-DU-ID</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>INTEGER (0..68719476735)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>68719476735</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>NGENB-DU-ID</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>INTEGER (0..68719476735)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>68719476735</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>OCTET STRING (SIZE(3))</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ServiceLayerCause</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>OCTET STRING</t>
+        </is>
+      </c>
+      <c r="E14" s="1" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>TransactionID</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>INTEGER (0..255, ...)</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>255</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="E15" s="1" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
@@ -543,7 +883,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,17 +891,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="34" customWidth="1" min="1" max="1"/>
+    <col width="42" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="34" customWidth="1" min="3" max="3"/>
+    <col width="42" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
-    <col width="34" customWidth="1" min="5" max="5"/>
-    <col width="34" customWidth="1" min="6" max="6"/>
+    <col width="42" customWidth="1" min="5" max="5"/>
+    <col width="42" customWidth="1" min="6" max="6"/>
     <col width="13" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
     <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
+    <col width="23" customWidth="1" min="11" max="11"/>
+    <col width="11" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -620,32 +961,41 @@
           <t>Max_Value</t>
         </is>
       </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Enum_Item</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>E2connectionUpdate</t>
+          <t>Cause</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>E2connectionUpdate</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>Cause</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>protocolIEs</t>
+          <t>ricRequest</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>ProtocolIE-Container</t>
+          <t>CauseRICrequest</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -657,39 +1007,40 @@
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-IEs</t>
+          <t>Cause</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-IEs</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+          <t>Cause</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>id-TransactionID</t>
+          <t>ricService</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>TransactionID</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>reject</t>
-        </is>
-      </c>
+          <t>CauseRICservice</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
@@ -698,44 +1049,41 @@
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-IEs</t>
+          <t>Cause</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-IEs</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>Cause</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>id-E2connectionUpdateAdd</t>
+          <t>e2Node</t>
         </is>
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-List</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>reject</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+          <t>CauseE2node</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
           <t>1</t>
@@ -743,44 +1091,41 @@
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-IEs</t>
+          <t>Cause</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-IEs</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+          <t>Cause</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>id-E2connectionUpdateRemove</t>
+          <t>transport</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>E2connectionUpdateRemove-List</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>reject</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+          <t>CauseTransport</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>1</t>
@@ -788,44 +1133,41 @@
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-IEs</t>
+          <t>Cause</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-IEs</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
+          <t>Cause</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>id-E2connectionUpdateModify</t>
+          <t>protocol</t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-List</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>reject</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+          <t>CauseProtocol</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
           <t>1</t>
@@ -833,32 +1175,37 @@
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-Item</t>
+          <t>Cause</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-Item</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+          <t>Cause</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>tnlInformation</t>
+          <t>misc</t>
         </is>
       </c>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>TNLinformation</t>
+          <t>CauseMisc</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -870,32 +1217,37 @@
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-Item</t>
+          <t>Cause</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-Item</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
+          <t>Cause</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>tnlUsage</t>
+          <t>serviceLayer</t>
         </is>
       </c>
       <c r="F8" s="1" t="inlineStr">
         <is>
-          <t>TNLusage</t>
+          <t>CauseServiceLayer</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -907,39 +1259,36 @@
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-ItemIEs</t>
+          <t>CauseServiceLayer</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>SEQUENCE</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-ItemIEs</t>
+          <t>CauseServiceLayer</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>id-E2connectionUpdate-Item</t>
+          <t>serviceLayerCause</t>
         </is>
       </c>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-Item</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>ignore</t>
-        </is>
-      </c>
+          <t>ServiceLayerCause</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
@@ -948,52 +1297,50 @@
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-List</t>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SingleContainer</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-List</t>
+          <t>e2nodeComponentInterfaceType</t>
         </is>
       </c>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-ItemIEs</t>
+          <t>E2nodeComponentInterfaceType</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>maxofTNLA</t>
-        </is>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>E2connectionUpdateRemove-Item</t>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1003,18 +1350,18 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>E2connectionUpdateRemove-Item</t>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>tnlInformation</t>
+          <t>e2nodeComponentID</t>
         </is>
       </c>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>TNLinformation</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -1026,39 +1373,36 @@
       </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>E2connectionUpdateRemove-ItemIEs</t>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>SEQUENCE</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>E2connectionUpdateRemove-ItemIEs</t>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>id-E2connectionUpdateRemove-Item</t>
+          <t>e2nodeComponentConfigurationAck</t>
         </is>
       </c>
       <c r="F12" s="1" t="inlineStr">
         <is>
-          <t>E2connectionUpdateRemove-Item</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>ignore</t>
-        </is>
-      </c>
+          <t>E2nodeComponentConfigurationAck</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
@@ -1067,89 +1411,96 @@
       </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>E2connectionUpdateRemove-List</t>
+          <t>E2nodeComponentConfigAdditionAck-ItemIEs</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SingleContainer</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigAdditionAck-ItemIEs</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>E2connectionUpdateRemove-List</t>
+          <t>id-E2nodeComponentConfigAdditionAck-Item</t>
         </is>
       </c>
       <c r="F13" s="1" t="inlineStr">
         <is>
-          <t>E2connectionUpdateRemove-ItemIEs</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>maxofTNLA</t>
-        </is>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TNLinformation</t>
+          <t>E2nodeComponentConfigAdditionAck-List</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>TNLinformation</t>
-        </is>
-      </c>
+          <t>SingleContainer</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>tnlAddress</t>
+          <t>E2nodeComponentConfigAdditionAck-List</t>
         </is>
       </c>
       <c r="F14" s="1" t="inlineStr">
         <is>
-          <t>BIT STRING (SIZE(1..160,...)</t>
+          <t>E2nodeComponentConfigAdditionAck-ItemIEs</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>TNLinformation</t>
+          <t>E2nodeComponentConfigRemovalAck-Item</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1159,26 +1510,22 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>TNLinformation</t>
+          <t>E2nodeComponentConfigRemovalAck-Item</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>tnlPort</t>
+          <t>e2nodeComponentInterfaceType</t>
         </is>
       </c>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>BIT STRING (SIZE(16)</t>
+          <t>E2nodeComponentInterfaceType</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
           <t>1</t>
@@ -1186,6 +1533,2073 @@
       </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigRemovalAck-Item</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigRemovalAck-Item</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>e2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigRemovalAck-Item</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigRemovalAck-Item</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" s="1" t="inlineStr">
+        <is>
+          <t>e2nodeComponentConfigurationAck</t>
+        </is>
+      </c>
+      <c r="F17" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigurationAck</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigRemovalAck-ItemIEs</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigRemovalAck-ItemIEs</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" s="1" t="inlineStr">
+        <is>
+          <t>id-E2nodeComponentConfigRemovalAck-Item</t>
+        </is>
+      </c>
+      <c r="F18" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigRemovalAck-Item</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigRemovalAck-List</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SingleContainer</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigRemovalAck-List</t>
+        </is>
+      </c>
+      <c r="F19" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigRemovalAck-ItemIEs</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigUpdateAck-Item</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigUpdateAck-Item</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>e2nodeComponentInterfaceType</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceType</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigUpdateAck-Item</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigUpdateAck-Item</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" s="1" t="inlineStr">
+        <is>
+          <t>e2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="F21" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigUpdateAck-Item</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigUpdateAck-Item</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" s="1" t="inlineStr">
+        <is>
+          <t>e2nodeComponentConfigurationAck</t>
+        </is>
+      </c>
+      <c r="F22" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigurationAck</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigUpdateAck-ItemIEs</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigUpdateAck-ItemIEs</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" s="1" t="inlineStr">
+        <is>
+          <t>id-E2nodeComponentConfigUpdateAck-Item</t>
+        </is>
+      </c>
+      <c r="F23" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigUpdateAck-Item</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigUpdateAck-List</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>SingleContainer</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigUpdateAck-List</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigUpdateAck-ItemIEs</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigurationAck</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigurationAck</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" s="1" t="inlineStr">
+        <is>
+          <t>updateOutcome</t>
+        </is>
+      </c>
+      <c r="F25" s="1" t="inlineStr">
+        <is>
+          <t>ENUMERATED</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigurationAck</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigurationAck</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" s="1" t="inlineStr">
+        <is>
+          <t>failure</t>
+        </is>
+      </c>
+      <c r="F26" s="1" t="inlineStr">
+        <is>
+          <t>failure</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigurationAck</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigurationAck</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" s="1" t="inlineStr">
+        <is>
+          <t>failureCause</t>
+        </is>
+      </c>
+      <c r="F27" s="1" t="inlineStr">
+        <is>
+          <t>Cause</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E28" s="1" t="inlineStr">
+        <is>
+          <t>e2nodeComponentInterfaceTypeNG</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceNG</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E29" s="1" t="inlineStr">
+        <is>
+          <t>e2nodeComponentInterfaceTypeXn</t>
+        </is>
+      </c>
+      <c r="F29" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceXn</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E30" s="1" t="inlineStr">
+        <is>
+          <t>e2nodeComponentInterfaceTypeE1</t>
+        </is>
+      </c>
+      <c r="F30" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceE1</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E31" s="1" t="inlineStr">
+        <is>
+          <t>e2nodeComponentInterfaceTypeF1</t>
+        </is>
+      </c>
+      <c r="F31" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceF1</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E32" s="1" t="inlineStr">
+        <is>
+          <t>e2nodeComponentInterfaceTypeW1</t>
+        </is>
+      </c>
+      <c r="F32" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceW1</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E33" s="1" t="inlineStr">
+        <is>
+          <t>e2nodeComponentInterfaceTypeS1</t>
+        </is>
+      </c>
+      <c r="F33" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceS1</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E34" s="1" t="inlineStr">
+        <is>
+          <t>e2nodeComponentInterfaceTypeX2</t>
+        </is>
+      </c>
+      <c r="F34" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceX2</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceE1</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceE1</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" s="1" t="inlineStr">
+        <is>
+          <t>gNB-CU-UP-ID</t>
+        </is>
+      </c>
+      <c r="F35" s="1" t="inlineStr">
+        <is>
+          <t>GNB-CU-UP-ID</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceF1</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceF1</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" s="1" t="inlineStr">
+        <is>
+          <t>gNB-DU-ID</t>
+        </is>
+      </c>
+      <c r="F36" s="1" t="inlineStr">
+        <is>
+          <t>GNB-DU-ID</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceNG</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceNG</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" s="1" t="inlineStr">
+        <is>
+          <t>amf-name</t>
+        </is>
+      </c>
+      <c r="F37" s="1" t="inlineStr">
+        <is>
+          <t>AMFName</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceS1</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceS1</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" s="1" t="inlineStr">
+        <is>
+          <t>mme-name</t>
+        </is>
+      </c>
+      <c r="F38" s="1" t="inlineStr">
+        <is>
+          <t>MMEname</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceW1</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceW1</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" s="1" t="inlineStr">
+        <is>
+          <t>ng-eNB-DU-ID</t>
+        </is>
+      </c>
+      <c r="F39" s="1" t="inlineStr">
+        <is>
+          <t>NGENB-DU-ID</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceX2</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceX2</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" s="1" t="inlineStr">
+        <is>
+          <t>global-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F40" s="1" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceX2</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceX2</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" s="1" t="inlineStr">
+        <is>
+          <t>global-en-gNB-ID</t>
+        </is>
+      </c>
+      <c r="F41" s="1" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceXn</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceXn</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" s="1" t="inlineStr">
+        <is>
+          <t>global-NG-RAN-Node-ID</t>
+        </is>
+      </c>
+      <c r="F42" s="1" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>E2nodeConfigurationUpdateAcknowledge</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>E2nodeConfigurationUpdateAcknowledge</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" s="1" t="inlineStr">
+        <is>
+          <t>protocolIEs</t>
+        </is>
+      </c>
+      <c r="F43" s="1" t="inlineStr">
+        <is>
+          <t>ProtocolIE-Container</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>E2nodeConfigurationUpdateAcknowledge-IEs</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>E2nodeConfigurationUpdateAcknowledge-IEs</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" s="1" t="inlineStr">
+        <is>
+          <t>id-TransactionID</t>
+        </is>
+      </c>
+      <c r="F44" s="1" t="inlineStr">
+        <is>
+          <t>TransactionID</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>E2nodeConfigurationUpdateAcknowledge-IEs</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>E2nodeConfigurationUpdateAcknowledge-IEs</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" s="1" t="inlineStr">
+        <is>
+          <t>id-E2nodeComponentConfigAdditionAck</t>
+        </is>
+      </c>
+      <c r="F45" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigAdditionAck-List</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>E2nodeConfigurationUpdateAcknowledge-IEs</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>E2nodeConfigurationUpdateAcknowledge-IEs</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" s="1" t="inlineStr">
+        <is>
+          <t>id-E2nodeComponentConfigUpdateAck</t>
+        </is>
+      </c>
+      <c r="F46" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigUpdateAck-List</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>E2nodeConfigurationUpdateAcknowledge-IEs</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>E2nodeConfigurationUpdateAcknowledge-IEs</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" s="1" t="inlineStr">
+        <is>
+          <t>id-E2nodeComponentConfigRemovalAck</t>
+        </is>
+      </c>
+      <c r="F47" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigRemovalAck-List</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E48" s="1" t="inlineStr">
+        <is>
+          <t>macro-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F48" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE (20)</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E49" s="1" t="inlineStr">
+        <is>
+          <t>home-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F49" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE (28)</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E50" s="1" t="inlineStr">
+        <is>
+          <t>short-Macro-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F50" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(18)</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E51" s="1" t="inlineStr">
+        <is>
+          <t>long-Macro-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F51" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(21)</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E52" s="1" t="inlineStr">
+        <is>
+          <t>enb-ID-macro</t>
+        </is>
+      </c>
+      <c r="F52" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(20)</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E53" s="1" t="inlineStr">
+        <is>
+          <t>enb-ID-shortmacro</t>
+        </is>
+      </c>
+      <c r="F53" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(18)</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E54" s="1" t="inlineStr">
+        <is>
+          <t>enb-ID-longmacro</t>
+        </is>
+      </c>
+      <c r="F54" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(21)</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>ENGNB-ID</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>ENGNB-ID</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E55" s="1" t="inlineStr">
+        <is>
+          <t>gNB-ID</t>
+        </is>
+      </c>
+      <c r="F55" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE (22..32)</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>GNB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>GNB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E56" s="1" t="inlineStr">
+        <is>
+          <t>gnb-ID</t>
+        </is>
+      </c>
+      <c r="F56" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(22..32)</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" s="1" t="inlineStr">
+        <is>
+          <t>pLMN-Identity</t>
+        </is>
+      </c>
+      <c r="F57" s="1" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" s="1" t="inlineStr">
+        <is>
+          <t>eNB-ID</t>
+        </is>
+      </c>
+      <c r="F58" s="1" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E59" s="1" t="inlineStr">
+        <is>
+          <t>gNB</t>
+        </is>
+      </c>
+      <c r="F59" s="1" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E60" s="1" t="inlineStr">
+        <is>
+          <t>ng-eNB</t>
+        </is>
+      </c>
+      <c r="F60" s="1" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" s="1" t="inlineStr">
+        <is>
+          <t>pLMN-Identity</t>
+        </is>
+      </c>
+      <c r="F61" s="1" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" s="1" t="inlineStr">
+        <is>
+          <t>gNB-ID</t>
+        </is>
+      </c>
+      <c r="F62" s="1" t="inlineStr">
+        <is>
+          <t>ENGNB-ID</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" s="1" t="inlineStr">
+        <is>
+          <t>plmn-id</t>
+        </is>
+      </c>
+      <c r="F63" s="1" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" s="1" t="inlineStr">
+        <is>
+          <t>gnb-id</t>
+        </is>
+      </c>
+      <c r="F64" s="1" t="inlineStr">
+        <is>
+          <t>GNB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" s="1" t="inlineStr">
+        <is>
+          <t>plmn-id</t>
+        </is>
+      </c>
+      <c r="F65" s="1" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" s="1" t="inlineStr">
+        <is>
+          <t>enb-id</t>
+        </is>
+      </c>
+      <c r="F66" s="1" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
+      <c r="L66" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1206,11 +3620,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="37" customWidth="1" min="2" max="2"/>
-    <col width="31" customWidth="1" min="3" max="3"/>
-    <col width="29" customWidth="1" min="4" max="4"/>
-    <col width="24" customWidth="1" min="5" max="5"/>
+    <col width="38" customWidth="1" min="1" max="1"/>
+    <col width="45" customWidth="1" min="2" max="2"/>
+    <col width="39" customWidth="1" min="3" max="3"/>
+    <col width="37" customWidth="1" min="4" max="4"/>
+    <col width="42" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
     <col width="11" customWidth="1" min="7" max="7"/>
   </cols>
@@ -1255,7 +3669,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>E2connectionUpdate</t>
+          <t>E2nodeConfigurationUpdateAcknowledge</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1275,7 +3689,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-IEs</t>
+          <t>E2nodeConfigurationUpdateAcknowledge-IEs</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1292,27 +3706,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>E2connectionUpdate</t>
+          <t>E2nodeConfigurationUpdateAcknowledge</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ID_id_E2connectionUpdate-List</t>
+          <t>ID_id_E2nodeComponentConfigAdditionAck-List</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-List</t>
+          <t>E2nodeComponentConfigAdditionAck-List</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>id-E2connectionUpdateAdd</t>
+          <t>id-E2nodeComponentConfigAdditionAck</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-IEs</t>
+          <t>E2nodeConfigurationUpdateAcknowledge-IEs</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1329,27 +3743,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>E2connectionUpdate</t>
+          <t>E2nodeConfigurationUpdateAcknowledge</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ID_id_E2connectionUpdateRemove-List</t>
+          <t>ID_id_E2nodeComponentConfigUpdateAck-List</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>E2connectionUpdateRemove-List</t>
+          <t>E2nodeComponentConfigUpdateAck-List</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>id-E2connectionUpdateRemove</t>
+          <t>id-E2nodeComponentConfigUpdateAck</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-IEs</t>
+          <t>E2nodeConfigurationUpdateAcknowledge-IEs</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1366,27 +3780,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>E2connectionUpdate</t>
+          <t>E2nodeConfigurationUpdateAcknowledge</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ID_id_E2connectionUpdate-List</t>
+          <t>ID_id_E2nodeComponentConfigRemovalAck-List</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-List</t>
+          <t>E2nodeComponentConfigRemovalAck-List</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>id-E2connectionUpdateModify</t>
+          <t>id-E2nodeComponentConfigRemovalAck</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>E2connectionUpdate-IEs</t>
+          <t>E2nodeConfigurationUpdateAcknowledge-IEs</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">

</xml_diff>